<commit_message>
Thao tác với bộ từ và từ khá ok
</commit_message>
<xml_diff>
--- a/src/data/dataFile/xlsx/Region Of Viet Nam.xlsx
+++ b/src/data/dataFile/xlsx/Region Of Viet Nam.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>English</t>
   </si>
@@ -54,12 +54,6 @@
   </si>
   <si>
     <t>nam trung bộ</t>
-  </si>
-  <si>
-    <t>the north</t>
-  </si>
-  <si>
-    <t>miền bắc</t>
   </si>
   <si>
     <t>the mekong river delta</t>
@@ -320,20 +314,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>